<commit_message>
Add Users sheet to Excel templates
</commit_message>
<xml_diff>
--- a/templates/combined-import-template.xlsx
+++ b/templates/combined-import-template.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet name="Appliances" sheetId="1" r:id="rId1"/>
     <sheet name="Fuels" sheetId="2" r:id="rId2"/>
+    <sheet name="Users" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -749,4 +750,108 @@
     <ignoredError numberStoredAsText="1" sqref="A1:W2"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" customWidth="1"/>
+    <col min="8" max="8" width="30.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>userId</v>
+      </c>
+      <c r="B1" t="str">
+        <v>firstName</v>
+      </c>
+      <c r="C1" t="str">
+        <v>lastName</v>
+      </c>
+      <c r="D1" t="str">
+        <v>email</v>
+      </c>
+      <c r="E1" t="str">
+        <v>phone</v>
+      </c>
+      <c r="F1" t="str">
+        <v>role</v>
+      </c>
+      <c r="G1" t="str">
+        <v>organization</v>
+      </c>
+      <c r="H1" t="str">
+        <v>address</v>
+      </c>
+      <c r="I1" t="str">
+        <v>city</v>
+      </c>
+      <c r="J1" t="str">
+        <v>postcode</v>
+      </c>
+      <c r="K1" t="str">
+        <v>isActive</v>
+      </c>
+      <c r="L1" t="str">
+        <v>registrationDate</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>USER001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Alex</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Smith</v>
+      </c>
+      <c r="D2" t="str">
+        <v>alex.smith@example.com</v>
+      </c>
+      <c r="E2" t="str">
+        <v>07123456789</v>
+      </c>
+      <c r="F2" t="str">
+        <v>user</v>
+      </c>
+      <c r="G2" t="str">
+        <v>Example Org</v>
+      </c>
+      <c r="H2" t="str">
+        <v>10 Example Street</v>
+      </c>
+      <c r="I2" t="str">
+        <v>Newcastle</v>
+      </c>
+      <c r="J2" t="str">
+        <v>NE1 1AA</v>
+      </c>
+      <c r="K2" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="L2" t="str">
+        <v>01/01/2025</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add relationship sheets to Excel templates
</commit_message>
<xml_diff>
--- a/templates/combined-import-template.xlsx
+++ b/templates/combined-import-template.xlsx
@@ -6,6 +6,8 @@
     <sheet name="Appliances" sheetId="1" r:id="rId1"/>
     <sheet name="Fuels" sheetId="2" r:id="rId2"/>
     <sheet name="Users" sheetId="3" r:id="rId3"/>
+    <sheet name="UserAppliances" sheetId="4" r:id="rId4"/>
+    <sheet name="UserFuels" sheetId="5" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
@@ -854,4 +856,114 @@
     <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="40.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>userId</v>
+      </c>
+      <c r="B1" t="str">
+        <v>applianceId</v>
+      </c>
+      <c r="C1" t="str">
+        <v>assignedDate</v>
+      </c>
+      <c r="D1" t="str">
+        <v>status</v>
+      </c>
+      <c r="E1" t="str">
+        <v>notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>USER001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>APP001</v>
+      </c>
+      <c r="C2" t="str">
+        <v>15/01/2025</v>
+      </c>
+      <c r="D2" t="str">
+        <v>active</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Primary heating appliance</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="40.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>userId</v>
+      </c>
+      <c r="B1" t="str">
+        <v>fuelId</v>
+      </c>
+      <c r="C1" t="str">
+        <v>assignedDate</v>
+      </c>
+      <c r="D1" t="str">
+        <v>status</v>
+      </c>
+      <c r="E1" t="str">
+        <v>notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>USER001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>FUEL001</v>
+      </c>
+      <c r="C2" t="str">
+        <v>15/01/2025</v>
+      </c>
+      <c r="D2" t="str">
+        <v>active</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Preferred fuel type</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>